<commit_message>
con't fixing mapping material inspection data
</commit_message>
<xml_diff>
--- a/material_data_output.xlsx
+++ b/material_data_output.xlsx
@@ -7,11 +7,11 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="EM0580107P" sheetId="1" r:id="rId1"/>
+    <sheet name="DFB6600600" sheetId="1" r:id="rId1"/>
     <sheet name="FM05000102-01A" sheetId="2" r:id="rId2"/>
-    <sheet name="DFB6600600" sheetId="3" r:id="rId3"/>
-    <sheet name="RDB5200200" sheetId="4" r:id="rId4"/>
-    <sheet name="EM0580106P" sheetId="5" r:id="rId5"/>
+    <sheet name="EM0580106P" sheetId="3" r:id="rId3"/>
+    <sheet name="EM0580107P" sheetId="4" r:id="rId4"/>
+    <sheet name="RDB5200200" sheetId="5" r:id="rId5"/>
     <sheet name="Inspection_Data" sheetId="6" r:id="rId6"/>
     <sheet name="Database_Data" sheetId="7" r:id="rId7"/>
   </sheets>
@@ -25,21 +25,177 @@
     <t>Column</t>
   </si>
   <si>
+    <t>Database_Average_DFB6600600_Value</t>
+  </si>
+  <si>
+    <t>DFB6600600_Value</t>
+  </si>
+  <si>
+    <t>Deviation</t>
+  </si>
+  <si>
+    <t>Matched_Inspection_Column</t>
+  </si>
+  <si>
+    <t>Matching_Strategy</t>
+  </si>
+  <si>
+    <t>Process_2_Df_Blk_Inspection_3_Average_Data</t>
+  </si>
+  <si>
+    <t>Process_2_Df_Blk_Inspection_3_Minimum_Data</t>
+  </si>
+  <si>
+    <t>Process_2_Df_Blk_Inspection_3_Maximum_Data</t>
+  </si>
+  <si>
+    <t>Process_2_Df_Blk_Inspection_4_Average_Data</t>
+  </si>
+  <si>
+    <t>Process_2_Df_Blk_Inspection_4_Minimum_Data</t>
+  </si>
+  <si>
+    <t>Process_2_Df_Blk_Inspection_4_Maximum_Data</t>
+  </si>
+  <si>
+    <t>Inspection_3_Resistance_Average</t>
+  </si>
+  <si>
+    <t>Inspection_3_Resistance_Minimum</t>
+  </si>
+  <si>
+    <t>Inspection_3_Resistance_Maximum</t>
+  </si>
+  <si>
+    <t>Inspection_4_Dimension_Average</t>
+  </si>
+  <si>
+    <t>Inspection_4_Dimension_Minimum</t>
+  </si>
+  <si>
+    <t>Inspection_4_Dimension_Maximum</t>
+  </si>
+  <si>
+    <t>Direct Material Mapping</t>
+  </si>
+  <si>
+    <t>Database_Average_FM05000102-01A_Value</t>
+  </si>
+  <si>
+    <t>FM05000102-01A_Value</t>
+  </si>
+  <si>
+    <t>Process_1_Frame_Inspection_3_Average_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Frame_Inspection_3_Minimum_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Frame_Inspection_3_Maximum_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Frame_Inspection_4_Average_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Frame_Inspection_4_Minimum_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Frame_Inspection_4_Maximum_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Frame_Inspection_5_Average_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Frame_Inspection_5_Minimum_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Frame_Inspection_5_Maximum_Data</t>
+  </si>
+  <si>
+    <t>Inspection_3_Average</t>
+  </si>
+  <si>
+    <t>Inspection_3_Minimum</t>
+  </si>
+  <si>
+    <t>Inspection_3_Maximum</t>
+  </si>
+  <si>
+    <t>Inspection_4_Average</t>
+  </si>
+  <si>
+    <t>Inspection_4_Minimum</t>
+  </si>
+  <si>
+    <t>Inspection_4_Maximum</t>
+  </si>
+  <si>
+    <t>Inspection_5_Average</t>
+  </si>
+  <si>
+    <t>Inspection_5_Minimum</t>
+  </si>
+  <si>
+    <t>Inspection_5_Maximum</t>
+  </si>
+  <si>
+    <t>Direct Frame Mapping</t>
+  </si>
+  <si>
+    <t>Database_Average_EM0580106P_Value</t>
+  </si>
+  <si>
+    <t>EM0580106P_Value</t>
+  </si>
+  <si>
+    <t>Process_1_Em2p_Inspection_10_Average_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Em2p_Inspection_3_Average_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Em2p_Inspection_3_Minimum_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Em2p_Inspection_3_Maximum_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Em2p_Inspection_4_Average_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Em2p_Inspection_4_Minimum_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Em2p_Inspection_4_Maximum_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Em2p_Inspection_5_Average_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Em2p_Inspection_5_Minimum_Data</t>
+  </si>
+  <si>
+    <t>Process_1_Em2p_Inspection_5_Maximum_Data</t>
+  </si>
+  <si>
+    <t>Inspection_10_Pull_Test</t>
+  </si>
+  <si>
+    <t>Inspection_5_Dimension_Average</t>
+  </si>
+  <si>
+    <t>Inspection_5_Dimension_Minimum</t>
+  </si>
+  <si>
+    <t>Inspection_5_Dimension_Maximum</t>
+  </si>
+  <si>
     <t>Database_Average_EM0580107P_Value</t>
   </si>
   <si>
     <t>EM0580107P_Value</t>
   </si>
   <si>
-    <t>Deviation</t>
-  </si>
-  <si>
-    <t>Matched_Inspection_Column</t>
-  </si>
-  <si>
-    <t>Matching_Strategy</t>
-  </si>
-  <si>
     <t>Process_1_Em3p_Inspection_10_Average_Data</t>
   </si>
   <si>
@@ -70,126 +226,6 @@
     <t>Process_1_Em3p_Inspection_5_Maximum_Data</t>
   </si>
   <si>
-    <t>Inspection_10_Pull_Test</t>
-  </si>
-  <si>
-    <t>Inspection_3_Resistance_Average</t>
-  </si>
-  <si>
-    <t>Inspection_3_Resistance_Minimum</t>
-  </si>
-  <si>
-    <t>Inspection_3_Resistance_Maximum</t>
-  </si>
-  <si>
-    <t>Inspection_4_Dimension_Average</t>
-  </si>
-  <si>
-    <t>Inspection_4_Dimension_Minimum</t>
-  </si>
-  <si>
-    <t>Inspection_4_Dimension_Maximum</t>
-  </si>
-  <si>
-    <t>Inspection_5_Dimension_Average</t>
-  </si>
-  <si>
-    <t>Inspection_5_Dimension_Minimum</t>
-  </si>
-  <si>
-    <t>Inspection_5_Dimension_Maximum</t>
-  </si>
-  <si>
-    <t>Direct Material Mapping</t>
-  </si>
-  <si>
-    <t>Database_Average_FM05000102-01A_Value</t>
-  </si>
-  <si>
-    <t>FM05000102-01A_Value</t>
-  </si>
-  <si>
-    <t>Process_1_Frame_Inspection_3_Average_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Frame_Inspection_3_Minimum_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Frame_Inspection_3_Maximum_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Frame_Inspection_4_Average_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Frame_Inspection_4_Minimum_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Frame_Inspection_4_Maximum_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Frame_Inspection_5_Average_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Frame_Inspection_5_Minimum_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Frame_Inspection_5_Maximum_Data</t>
-  </si>
-  <si>
-    <t>Inspection_3_Average</t>
-  </si>
-  <si>
-    <t>Inspection_3_Minimum</t>
-  </si>
-  <si>
-    <t>Inspection_3_Maximum</t>
-  </si>
-  <si>
-    <t>Inspection_4_Average</t>
-  </si>
-  <si>
-    <t>Inspection_4_Minimum</t>
-  </si>
-  <si>
-    <t>Inspection_4_Maximum</t>
-  </si>
-  <si>
-    <t>Inspection_5_Average</t>
-  </si>
-  <si>
-    <t>Inspection_5_Minimum</t>
-  </si>
-  <si>
-    <t>Inspection_5_Maximum</t>
-  </si>
-  <si>
-    <t>Direct Frame Mapping</t>
-  </si>
-  <si>
-    <t>Database_Average_DFB6600600_Value</t>
-  </si>
-  <si>
-    <t>DFB6600600_Value</t>
-  </si>
-  <si>
-    <t>Process_2_Df_Blk_Inspection_3_Average_Data</t>
-  </si>
-  <si>
-    <t>Process_2_Df_Blk_Inspection_3_Minimum_Data</t>
-  </si>
-  <si>
-    <t>Process_2_Df_Blk_Inspection_3_Maximum_Data</t>
-  </si>
-  <si>
-    <t>Process_2_Df_Blk_Inspection_4_Average_Data</t>
-  </si>
-  <si>
-    <t>Process_2_Df_Blk_Inspection_4_Minimum_Data</t>
-  </si>
-  <si>
-    <t>Process_2_Df_Blk_Inspection_4_Maximum_Data</t>
-  </si>
-  <si>
     <t>Database_Average_RDB5200200_Value</t>
   </si>
   <si>
@@ -221,42 +257,6 @@
   </si>
   <si>
     <t>Process_2_Rod_Blk_Inspection_5_Maximum_Data</t>
-  </si>
-  <si>
-    <t>Database_Average_EM0580106P_Value</t>
-  </si>
-  <si>
-    <t>EM0580106P_Value</t>
-  </si>
-  <si>
-    <t>Process_1_Em2p_Inspection_10_Average_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Em2p_Inspection_3_Average_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Em2p_Inspection_3_Minimum_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Em2p_Inspection_3_Maximum_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Em2p_Inspection_4_Average_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Em2p_Inspection_4_Minimum_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Em2p_Inspection_4_Maximum_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Em2p_Inspection_5_Average_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Em2p_Inspection_5_Minimum_Data</t>
-  </si>
-  <si>
-    <t>Process_1_Em2p_Inspection_5_Maximum_Data</t>
   </si>
   <si>
     <t>Material_Code</t>
@@ -2264,7 +2264,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2295,19 +2295,16 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>2.129999999999999</v>
-      </c>
-      <c r="C2">
-        <v>1.46</v>
+        <v>2.2</v>
       </c>
       <c r="D2">
-        <v>0.2441314553990608</v>
+        <v>0.5863636363636363</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2315,19 +2312,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.8999999999999999</v>
-      </c>
-      <c r="C3">
-        <v>0.91</v>
+        <v>2.19</v>
       </c>
       <c r="D3">
-        <v>-0.01111111111111125</v>
+        <v>0.5844748858447488</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2335,19 +2329,16 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.8799999999999999</v>
-      </c>
-      <c r="C4">
-        <v>0.9</v>
+        <v>2.21</v>
       </c>
       <c r="D4">
-        <v>-0.03409090909090925</v>
+        <v>0.5837104072398189</v>
       </c>
       <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2355,19 +2346,16 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.9400000000000001</v>
-      </c>
-      <c r="C5">
-        <v>0.91</v>
+        <v>7.07</v>
       </c>
       <c r="D5">
-        <v>0.02127659574468087</v>
+        <v>0.949080622347949</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2375,19 +2363,16 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.3699999999999999</v>
-      </c>
-      <c r="C6">
-        <v>0.34</v>
+        <v>7.050000000000001</v>
       </c>
       <c r="D6">
-        <v>0.02702702702702691</v>
+        <v>0.9546099290780141</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2395,99 +2380,16 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.3100000000000001</v>
-      </c>
-      <c r="C7">
-        <v>0.32</v>
+        <v>7.09</v>
       </c>
       <c r="D7">
-        <v>-0.03225806451612888</v>
+        <v>0.9421720733427362</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>0.48</v>
-      </c>
-      <c r="C8">
-        <v>0.38</v>
-      </c>
-      <c r="D8">
-        <v>0.1458333333333333</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>0.47</v>
-      </c>
-      <c r="C9">
-        <v>0.43</v>
-      </c>
-      <c r="D9">
-        <v>0.2127659574468086</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>0.34</v>
-      </c>
-      <c r="C10">
-        <v>0.38</v>
-      </c>
-      <c r="D10">
-        <v>0.05882352941176475</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>0.57</v>
-      </c>
-      <c r="C11">
-        <v>0.47</v>
-      </c>
-      <c r="D11">
-        <v>0.2807017543859649</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2508,10 +2410,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -2525,7 +2427,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>63.68882352941176</v>
@@ -2534,15 +2436,15 @@
         <v>0.9857117787773273</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>63.68470588235294</v>
@@ -2551,15 +2453,15 @@
         <v>0.9857108549471663</v>
       </c>
       <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>39</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>63.6964705882353</v>
@@ -2568,15 +2470,15 @@
         <v>0.9855564995751911</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>76.85470588235293</v>
@@ -2585,15 +2487,15 @@
         <v>0.9953158366053593</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>76.84</v>
@@ -2602,15 +2504,15 @@
         <v>0.99583550234253</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>76.86529411764707</v>
@@ -2619,15 +2521,15 @@
         <v>0.9946659932196127</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>63.67294117647058</v>
@@ -2636,15 +2538,15 @@
         <v>0.9941890543586712</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>63.65588235294118</v>
@@ -2653,15 +2555,15 @@
         <v>0.9949729704754424</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>63.67882352941177</v>
@@ -2670,10 +2572,10 @@
         <v>0.9935614388382877</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2683,7 +2585,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2694,10 +2596,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -2711,104 +2613,202 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B2">
-        <v>2.2</v>
+        <v>2.26</v>
+      </c>
+      <c r="C2">
+        <v>1.61</v>
       </c>
       <c r="D2">
-        <v>0.5863636363636363</v>
+        <v>0.2876106194690266</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B3">
-        <v>2.19</v>
+        <v>0.9200000000000002</v>
+      </c>
+      <c r="C3">
+        <v>0.91</v>
       </c>
       <c r="D3">
-        <v>0.5844748858447488</v>
+        <v>0.01086956521739143</v>
       </c>
       <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B4">
-        <v>2.21</v>
+        <v>0.8799999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.91</v>
       </c>
       <c r="D4">
-        <v>0.5837104072398189</v>
+        <v>-0.03409090909090925</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B5">
-        <v>7.07</v>
+        <v>0.9900000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.92</v>
       </c>
       <c r="D5">
-        <v>0.949080622347949</v>
+        <v>0.07070707070707076</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B6">
-        <v>7.050000000000001</v>
+        <v>0.4</v>
+      </c>
+      <c r="C6">
+        <v>0.36</v>
       </c>
       <c r="D6">
-        <v>0.9546099290780141</v>
+        <v>0.1000000000000001</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>0.3100000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.32</v>
+      </c>
+      <c r="D7">
+        <v>-0.03225806451612888</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <v>0.5300000000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.41</v>
+      </c>
+      <c r="D8">
+        <v>0.2264150943396229</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>0.4600000000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.37</v>
+      </c>
+      <c r="D9">
+        <v>0.1956521739130436</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <v>0.35</v>
+      </c>
+      <c r="C10">
+        <v>0.32</v>
+      </c>
+      <c r="D10">
+        <v>0.08571428571428563</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11">
+        <v>0.5599999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.41</v>
+      </c>
+      <c r="D11">
+        <v>0.2678571428571428</v>
+      </c>
+      <c r="E11" t="s">
         <v>55</v>
       </c>
-      <c r="B7">
-        <v>7.09</v>
-      </c>
-      <c r="D7">
-        <v>0.9421720733427362</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
+      <c r="F11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2817,6 +2817,239 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>2.129999999999999</v>
+      </c>
+      <c r="C2">
+        <v>1.46</v>
+      </c>
+      <c r="D2">
+        <v>0.2441314553990608</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.91</v>
+      </c>
+      <c r="D3">
+        <v>-0.01111111111111125</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>0.8799999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.9</v>
+      </c>
+      <c r="D4">
+        <v>-0.03409090909090925</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>0.9400000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.91</v>
+      </c>
+      <c r="D5">
+        <v>0.02127659574468087</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6">
+        <v>0.3699999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.34</v>
+      </c>
+      <c r="D6">
+        <v>0.02702702702702691</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7">
+        <v>0.3100000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.32</v>
+      </c>
+      <c r="D7">
+        <v>-0.03225806451612888</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8">
+        <v>0.48</v>
+      </c>
+      <c r="C8">
+        <v>0.38</v>
+      </c>
+      <c r="D8">
+        <v>0.1458333333333333</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9">
+        <v>0.47</v>
+      </c>
+      <c r="C9">
+        <v>0.43</v>
+      </c>
+      <c r="D9">
+        <v>0.2127659574468086</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10">
+        <v>0.34</v>
+      </c>
+      <c r="C10">
+        <v>0.38</v>
+      </c>
+      <c r="D10">
+        <v>0.05882352941176475</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11">
+        <v>0.57</v>
+      </c>
+      <c r="C11">
+        <v>0.47</v>
+      </c>
+      <c r="D11">
+        <v>0.2807017543859649</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -2829,10 +3062,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -2846,7 +3079,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <v>13.5</v>
@@ -2855,15 +3088,15 @@
         <v>0.9325925925925925</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B3">
         <v>13.48</v>
@@ -2872,15 +3105,15 @@
         <v>0.9324925816023739</v>
       </c>
       <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B4">
         <v>13.51</v>
@@ -2889,15 +3122,15 @@
         <v>0.9319022945965951</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B5">
         <v>7.940000000000001</v>
@@ -2906,15 +3139,15 @@
         <v>0.9546599496221662</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>7.93</v>
@@ -2923,15 +3156,15 @@
         <v>0.9596469104665826</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B7">
         <v>7.96</v>
@@ -2940,15 +3173,15 @@
         <v>0.9484924623115578</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B8">
         <v>7.93</v>
@@ -2957,15 +3190,15 @@
         <v>0.9533417402269861</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B9">
         <v>7.920000000000001</v>
@@ -2974,15 +3207,15 @@
         <v>0.9595959595959596</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B10">
         <v>7.95</v>
@@ -2991,243 +3224,10 @@
         <v>0.9484276729559749</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2">
-        <v>2.26</v>
-      </c>
-      <c r="C2">
-        <v>1.61</v>
-      </c>
-      <c r="D2">
-        <v>0.2876106194690266</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3">
-        <v>0.9200000000000002</v>
-      </c>
-      <c r="C3">
-        <v>0.91</v>
-      </c>
-      <c r="D3">
-        <v>0.01086956521739143</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4">
-        <v>0.8799999999999999</v>
-      </c>
-      <c r="C4">
-        <v>0.91</v>
-      </c>
-      <c r="D4">
-        <v>-0.03409090909090925</v>
-      </c>
-      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5">
-        <v>0.9900000000000001</v>
-      </c>
-      <c r="C5">
-        <v>0.92</v>
-      </c>
-      <c r="D5">
-        <v>0.07070707070707076</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6">
-        <v>0.4</v>
-      </c>
-      <c r="C6">
-        <v>0.36</v>
-      </c>
-      <c r="D6">
-        <v>0.1000000000000001</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7">
-        <v>0.3100000000000001</v>
-      </c>
-      <c r="C7">
-        <v>0.32</v>
-      </c>
-      <c r="D7">
-        <v>-0.03225806451612888</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8">
-        <v>0.5300000000000001</v>
-      </c>
-      <c r="C8">
-        <v>0.41</v>
-      </c>
-      <c r="D8">
-        <v>0.2264150943396229</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9">
-        <v>0.4600000000000001</v>
-      </c>
-      <c r="C9">
-        <v>0.37</v>
-      </c>
-      <c r="D9">
-        <v>0.1956521739130436</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10">
-        <v>0.35</v>
-      </c>
-      <c r="C10">
-        <v>0.32</v>
-      </c>
-      <c r="D10">
-        <v>0.08571428571428563</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11">
-        <v>0.5599999999999999</v>
-      </c>
-      <c r="C11">
-        <v>0.41</v>
-      </c>
-      <c r="D11">
-        <v>0.2678571428571428</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3254,34 +3254,34 @@
         <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>82</v>
@@ -3302,31 +3302,31 @@
         <v>87</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>88</v>
@@ -3553,34 +3553,34 @@
         <v>139</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>140</v>
@@ -3589,34 +3589,34 @@
         <v>141</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>142</v>
@@ -3637,13 +3637,13 @@
         <v>147</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>148</v>
@@ -3658,13 +3658,13 @@
         <v>151</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>152</v>
@@ -3679,13 +3679,13 @@
         <v>155</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>156</v>
@@ -3775,13 +3775,13 @@
         <v>184</v>
       </c>
       <c r="CB1" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="CE1" s="1" t="s">
         <v>185</v>
@@ -3802,13 +3802,13 @@
         <v>190</v>
       </c>
       <c r="CK1" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="CN1" s="1" t="s">
         <v>191</v>
@@ -3829,13 +3829,13 @@
         <v>196</v>
       </c>
       <c r="CT1" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="CU1" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="CW1" s="1" t="s">
         <v>197</v>
@@ -3862,10 +3862,10 @@
         <v>204</v>
       </c>
       <c r="DE1" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="DF1" s="1" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="DG1" s="1" t="s">
         <v>205</v>
@@ -3874,10 +3874,10 @@
         <v>206</v>
       </c>
       <c r="DI1" s="1" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="DJ1" s="1" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="DK1" s="1" t="s">
         <v>207</v>
@@ -3886,10 +3886,10 @@
         <v>208</v>
       </c>
       <c r="DM1" s="1" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="DN1" s="1" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="DO1" s="1" t="s">
         <v>209</v>

</xml_diff>